<commit_message>
Exercício sobre a Maquina de Turing
</commit_message>
<xml_diff>
--- a/Aula_14_(21-08-2025)/Maquina_de_Turing_Atividade_Aula_14.xlsx
+++ b/Aula_14_(21-08-2025)/Maquina_de_Turing_Atividade_Aula_14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\Desktop\Quarto_Semestre_Ciencia_de_Dados\Aula_14_(21-08-2025)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6967A-171F-4082-9EDC-84D691A55A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003E917E-91EA-4B2C-A9CB-094898305A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5A6B9747-B439-4F7C-8C1B-35C28A7CD812}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5A6B9747-B439-4F7C-8C1B-35C28A7CD812}"/>
   </bookViews>
   <sheets>
     <sheet name="101010" sheetId="3" r:id="rId1"/>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -194,6 +194,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -206,25 +218,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,7 +613,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -646,12 +643,12 @@
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -663,10 +660,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -696,12 +693,12 @@
       <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -713,10 +710,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="4"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="9"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -746,12 +743,12 @@
       <c r="J8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -763,10 +760,10 @@
       <c r="H9" s="1"/>
       <c r="I9" s="3"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="9"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="13">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -796,12 +793,12 @@
       <c r="J11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,7 +810,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -834,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09752E72-EFE9-46C1-8E22-00B0FB0DD346}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -855,7 +852,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -871,12 +868,12 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -884,10 +881,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="9"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -903,12 +900,12 @@
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -916,10 +913,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="7"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -935,12 +932,12 @@
       <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,10 +945,10 @@
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -961,18 +958,18 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -980,10 +977,10 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="13">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -995,18 +992,18 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="11">
-        <v>0</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,10 +1011,10 @@
       <c r="D15" s="2"/>
       <c r="E15" s="6"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="13">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1029,18 +1026,18 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="11">
-        <v>0</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1048,10 +1045,10 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="16">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1063,18 +1060,18 @@
       <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1082,10 +1079,16 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="10"/>
+      <c r="G21" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A5:A6"/>
@@ -1094,12 +1097,6 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="G17:G18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1107,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703D1DFB-6330-42B2-85A9-3BA0850AF495}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,7 +1127,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1154,12 +1151,12 @@
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1169,10 +1166,10 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1196,12 +1193,12 @@
       <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1211,10 +1208,10 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1238,12 +1235,12 @@
       <c r="H8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1253,10 +1250,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1280,25 +1277,25 @@
       <c r="H11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="13">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1322,79 +1319,79 @@
       <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
-        <v>7</v>
-      </c>
+      <c r="A18" s="16"/>
       <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="12">
-        <v>1</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="I14:I15"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="I8:I9"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="I14:I15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1402,15 +1399,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B35F515-10C8-4726-A2FF-E8AC7D3B6D6D}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54:G54"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.5546875" customWidth="1"/>
     <col min="4" max="8" width="2.21875" customWidth="1"/>
     <col min="9" max="11" width="2" bestFit="1" customWidth="1"/>
@@ -1418,7 +1415,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
@@ -1426,7 +1423,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1457,12 +1454,12 @@
       <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1475,10 +1472,10 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="9"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1509,12 +1506,12 @@
       <c r="K5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1527,10 +1524,10 @@
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1561,12 +1558,12 @@
       <c r="K8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1579,10 +1576,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="7"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1613,877 +1610,836 @@
       <c r="K11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
-        <v>5</v>
-      </c>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="7" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="6"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="6"/>
-      <c r="L16" s="7"/>
-    </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
-        <v>6</v>
-      </c>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="7" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="J19" s="10"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="16"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-      <c r="L20" s="15"/>
-    </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
-        <v>7</v>
-      </c>
+      <c r="A21" s="18"/>
       <c r="B21" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L21" s="7" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="J22" s="10"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="16"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-      <c r="L23" s="15"/>
-    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
-        <v>8</v>
-      </c>
+      <c r="A24" s="18"/>
       <c r="B24" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="7" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="J25" s="10"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="J28" s="10"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="J31" s="10"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="15"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="19">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>13</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
+        <v>14</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>15</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>16</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="18">
+        <v>17</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="13"/>
+    </row>
+    <row r="52" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="17">
+        <v>18</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L53" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="15"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="19">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="15"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="19">
-        <v>11</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1">
-        <v>0</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L33" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="7"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
-        <v>12</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
-      <c r="J36" s="1">
-        <v>0</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="7"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="19">
-        <v>13</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0</v>
-      </c>
-      <c r="J39" s="1">
-        <v>0</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="7"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="19">
-        <v>14</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0</v>
-      </c>
-      <c r="J42" s="1">
-        <v>0</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L42" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="7"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
-        <v>15</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0</v>
-      </c>
-      <c r="J45" s="1">
-        <v>0</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
-      <c r="B46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="7"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="19">
-        <v>16</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
-        <v>0</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L48" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
-      <c r="B49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="7"/>
-    </row>
-    <row r="50" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="19">
-        <v>17</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-      <c r="F51" s="1">
-        <v>0</v>
-      </c>
-      <c r="G51" s="1">
-        <v>0</v>
-      </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-      <c r="I51" s="1">
-        <v>0</v>
-      </c>
-      <c r="J51" s="1">
-        <v>0</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L51" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="7"/>
-    </row>
-    <row r="53" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="21">
-        <v>18</v>
-      </c>
+      <c r="A54" s="17"/>
       <c r="B54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0</v>
-      </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>0</v>
-      </c>
-      <c r="J54" s="2">
-        <v>0</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L54" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
-      <c r="B55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="L18:L19"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="L38:L39"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2515,7 +2471,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2545,12 +2501,12 @@
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2562,10 +2518,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2595,12 +2551,12 @@
       <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2612,10 +2568,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="7"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2645,12 +2601,12 @@
       <c r="J8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2662,11 +2618,11 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="16">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2696,12 +2652,12 @@
       <c r="J11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2713,7 +2669,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2734,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045BD7EF-C5F7-4749-806A-15F0FA5F0FE0}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:R2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,7 +2713,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2811,12 +2767,12 @@
       <c r="R2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2827,19 +2783,19 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="9"/>
+      <c r="S3" s="15"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2893,12 +2849,12 @@
       <c r="R5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2908,20 +2864,20 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="7"/>
+      <c r="S6" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2975,12 +2931,12 @@
       <c r="R8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="S8" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2991,20 +2947,20 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="7"/>
+      <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:19" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="16">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3058,12 +3014,12 @@
       <c r="R11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="S11" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
@@ -3083,7 +3039,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="10"/>
+      <c r="S12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3101,15 +3057,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100558A873A104A224C976CED04B936EDA0" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="96e23ddf523fdce0b9f32f10667b7dfb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c508f87f-076a-48e0-a84d-082a67831f97" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="18f1eb99c62998dd44352f297a76fc4a" ns2:_="">
     <xsd:import namespace="c508f87f-076a-48e0-a84d-082a67831f97"/>
@@ -3267,6 +3214,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3274,14 +3230,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F9BBF1-7C48-4979-8C56-5547E7D8DB65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2A88B56-D646-4E5E-9F73-F36D078F35B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3299,6 +3247,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F9BBF1-7C48-4979-8C56-5547E7D8DB65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EDD360-4916-4B09-BF4C-241C91F92C79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Atividade Aula 14 - Exercício sobre a Maquina de Turing
</commit_message>
<xml_diff>
--- a/Aula_14_(21-08-2025)/Maquina_de_Turing_Atividade_Aula_14.xlsx
+++ b/Aula_14_(21-08-2025)/Maquina_de_Turing_Atividade_Aula_14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\Desktop\Quarto_Semestre_Ciencia_de_Dados\Aula_14_(21-08-2025)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\Desktop\GitHub\Quarto_Semestre_Ciencia_de_Dados\Aula_14_(21-08-2025)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D10127-874E-43AE-BD6C-5A6828B99DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7086A934-56DB-4C5D-AF26-600D97BFB134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5A6B9747-B439-4F7C-8C1B-35C28A7CD812}"/>
   </bookViews>
@@ -219,10 +219,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,7 +832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD8682B-C540-4A3F-8436-5A51B72946FB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1095,6 +1097,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A5:A6"/>
@@ -1103,12 +1111,6 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="G17:G18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1390,18 +1392,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="I14:I15"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1431,7 +1433,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1467,7 +1469,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1485,7 @@
       <c r="L3" s="15"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="18">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1519,7 +1521,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1535,7 +1537,7 @@
       <c r="L6" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="A8" s="18">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1571,7 +1573,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1587,7 +1589,7 @@
       <c r="L9" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="18">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1623,7 +1625,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1639,7 +1641,7 @@
       <c r="L12" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="18">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1675,7 +1677,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1692,7 @@
       <c r="L15" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="18">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1726,7 +1728,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1747,7 +1749,7 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="17">
+      <c r="A20" s="18">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1783,7 +1785,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1804,7 +1806,7 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="18">
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1840,7 +1842,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1861,7 +1863,7 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
+      <c r="A26" s="18">
         <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1897,7 +1899,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1918,7 +1920,7 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="17">
+      <c r="A29" s="18">
         <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1956,7 +1958,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1977,7 +1979,7 @@
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="17">
+      <c r="A32" s="18">
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2015,7 +2017,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
@@ -2031,7 +2033,7 @@
       <c r="L33" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="17">
+      <c r="A35" s="18">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2069,7 +2071,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2085,7 +2087,7 @@
       <c r="L36" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="17">
+      <c r="A38" s="18">
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2123,7 +2125,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
@@ -2139,7 +2141,7 @@
       <c r="L39" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="17">
+      <c r="A41" s="18">
         <v>14</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2177,7 +2179,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
@@ -2193,7 +2195,7 @@
       <c r="L42" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="17">
+      <c r="A44" s="18">
         <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2231,7 +2233,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
@@ -2247,7 +2249,7 @@
       <c r="L45" s="13"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="17">
+      <c r="A47" s="18">
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2285,7 +2287,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2304,7 @@
     </row>
     <row r="49" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="17">
+      <c r="A50" s="18">
         <v>17</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2340,7 +2342,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
@@ -2357,7 +2359,7 @@
     </row>
     <row r="52" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="18">
+      <c r="A53" s="17">
         <v>18</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2395,7 +2397,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2412,6 +2414,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="L32:L33"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="L53:L54"/>
     <mergeCell ref="A26:A27"/>
@@ -2428,26 +2450,6 @@
     <mergeCell ref="L35:L36"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="L38:L39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3220,18 +3222,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3253,18 +3255,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F9BBF1-7C48-4979-8C56-5547E7D8DB65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EDD360-4916-4B09-BF4C-241C91F92C79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55F9BBF1-7C48-4979-8C56-5547E7D8DB65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>